<commit_message>
- added topological sorter to make dag for rating order - added multiprocessing to rate multiple rating steps concurrently - tested on WGIC rating plan and it works!
</commit_message>
<xml_diff>
--- a/examples/WGIC/WGIC_rating_manual.xlsx
+++ b/examples/WGIC/WGIC_rating_manual.xlsx
@@ -5,17 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="base_rates" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="amount_of_insurance_factor" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="territory_factor" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="protectionclass_constructiontyp" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="protectclass_constr_factor" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="underwriting_tier_factor" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="deductible_factor" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="new_home_discount_factor" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="five_year_claim_free_discount_f" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="five_year_claim_free_factor" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="multi_policy_discount_factor" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -210,7 +210,7 @@
       <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -251,9 +251,9 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.83"/>
   </cols>
   <sheetData>
@@ -2549,7 +2549,7 @@
       <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2640,11 +2640,11 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.46"/>
   </cols>
@@ -2985,7 +2985,7 @@
       <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3068,7 +3068,7 @@
       <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3151,7 +3151,7 @@
       <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3212,7 +3212,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3269,11 +3269,11 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.46"/>
   </cols>

</xml_diff>

<commit_message>
- Separated subclassing of pd.DataFrame and pd.Series into base.py, overloading some opeartors. - working Metromile rate plan!
</commit_message>
<xml_diff>
--- a/examples/WGIC/WGIC_rating_manual.xlsx
+++ b/examples/WGIC/WGIC_rating_manual.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="base_rates" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
   <si>
     <t xml:space="preserve">BI_</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t xml:space="preserve">_new_home_discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">_five_year_claim_free_discount</t>
@@ -183,7 +189,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -207,10 +213,10 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="J33"/>
+      <selection pane="topLeft" activeCell="J33" activeCellId="1" sqref="A2:A3 J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -248,10 +254,10 @@
   <dimension ref="A1:F663"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="A2:A3 E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.83"/>
@@ -2546,10 +2552,10 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
+      <selection pane="topLeft" activeCell="B52" activeCellId="1" sqref="A2:A3 B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2640,11 +2646,11 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="1" sqref="A2:A3 D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.46"/>
   </cols>
@@ -2982,10 +2988,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
+      <selection pane="topLeft" activeCell="L18" activeCellId="1" sqref="A2:A3 L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3065,10 +3071,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+      <selection pane="topLeft" activeCell="G34" activeCellId="1" sqref="A2:A3 G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3148,10 +3154,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3165,9 +3171,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="A2" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0.8</v>
@@ -3178,9 +3183,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A3" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
@@ -3209,14 +3213,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3226,9 +3230,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="A2" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0.9</v>
@@ -3239,9 +3242,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A3" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>
@@ -3269,18 +3271,18 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3290,9 +3292,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="A2" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0.93</v>
@@ -3303,9 +3304,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="A3" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1</v>

</xml_diff>